<commit_message>
Added non-linear grip and load sensitivity
Non-linear grip decreases the amount of grip with more load. Resulted in lap times being slower, which makes sense. Added graph in a new excel file and you can see the peak force it is levelling out at is much lower than before. Also added load sensitivity. If below a threshold then stiffness increases (more responsive/sharp) and if above it decreases (more sluggish/lazy). Also makes lap times slower, so it is difficult to get below a 48.5 now. Could need to add more downforce, as Imola is a high downforce circuit and I just stole the values off of the internet not specifying a set up, so possible the downforce values are just kind of an average middle of the road set up. I know in the turn before Acque Minerali real cars/other sims can go maybe 128-130kmh, and I think I can go about 105 and still actually make the corner. So I need more grip but I still don't spin up the tires when flooring the throttle from a stand still.
</commit_message>
<xml_diff>
--- a/FullBrushTireForces.xlsx
+++ b/FullBrushTireForces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JamesEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DE186B-A466-495A-8611-985154DC7D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093B0D6D-5B68-4110-8F2D-08FF114849ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{69B88305-7471-4B29-B417-11FB95EBCF15}"/>
   </bookViews>
@@ -2188,7 +2188,7 @@
   <dimension ref="A1:B151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V44" sqref="V44"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>